<commit_message>
Added secure feature changes
</commit_message>
<xml_diff>
--- a/logs/sessions/session_18eb340f24d94c1883fc69d061bb0824.xlsx
+++ b/logs/sessions/session_18eb340f24d94c1883fc69d061bb0824.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -761,7 +761,197 @@
           <t>Mozilla/5.0 (Macintosh; Intel Mac OS X 10_15_7) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/138.0.0.0 Safari/537.36</t>
         </is>
       </c>
-      <c r="I9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2025-12-11T04:52:35.466358</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>sunil</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>2</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>GET</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="F10" t="n">
+        <v>200</v>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>127.0.0.1</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (Macintosh; Intel Mac OS X 10_15_7) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/138.0.0.0 Safari/537.36</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2025-12-11T04:52:35.524407</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>sunil</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>2</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>GET</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>/favicon.ico</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
+        <v>404</v>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>127.0.0.1</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (Macintosh; Intel Mac OS X 10_15_7) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/138.0.0.0 Safari/537.36</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2025-12-11T04:52:38.886638</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>sunil</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>2</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>GET</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>/docs</t>
+        </is>
+      </c>
+      <c r="F12" t="n">
+        <v>200</v>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>127.0.0.1</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (Macintosh; Intel Mac OS X 10_15_7) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/138.0.0.0 Safari/537.36</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2025-12-11T04:52:39.039368</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>sunil</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>2</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>GET</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>/openapi.json</t>
+        </is>
+      </c>
+      <c r="F13" t="n">
+        <v>200</v>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>127.0.0.1</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (Macintosh; Intel Mac OS X 10_15_7) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/138.0.0.0 Safari/537.36</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2025-12-11T04:53:58.648374</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>sunil</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>2</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>POST</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>/auth/secure-login</t>
+        </is>
+      </c>
+      <c r="F14" t="n">
+        <v>200</v>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>127.0.0.1</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (Macintosh; Intel Mac OS X 10_15_7) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/138.0.0.0 Safari/537.36</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>